<commit_message>
Fix custom xml for 2EXT02_ProteomicsExtraction.
</commit_message>
<xml_diff>
--- a/templates/2EXT02_ProteomicsExtraction/2EXT02_ProteomicsExtraction.xlsx
+++ b/templates/2EXT02_ProteomicsExtraction/2EXT02_ProteomicsExtraction.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/630acb9a9506da97/CSB-Stuff/NFDI/ProteomicsTemplate/modular/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Freym\source\repos\SWATE_templates\templates\2EXT02_ProteomicsExtraction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="121" documentId="8_{4E2E7680-CDC8-425A-8327-0918921D25A2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{3CEA24FC-289F-4210-8966-9036AFD4543B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCFEC1F8-DCDA-46F0-BC27-603ABCD0AECD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B0FB3F19-C527-41AF-B02D-0669FBE7650F}"/>
+    <workbookView xWindow="-20055" yWindow="-5760" windowWidth="9120" windowHeight="5715" xr2:uid="{B0FB3F19-C527-41AF-B02D-0669FBE7650F}"/>
   </bookViews>
   <sheets>
     <sheet name="2EXT02_ProteomicsExtraction" sheetId="8" r:id="rId1"/>
@@ -50,25 +50,25 @@
   <commentList>
     <comment ref="A1" authorId="0" shapeId="0" xr:uid="{3A0AD166-FBB2-4AB6-96A6-A464A626EC8F}">
       <text>
-        <t>[Kommentarthread]
-Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
-Kommentar:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     (previously known as)</t>
       </text>
     </comment>
     <comment ref="H1" authorId="1" shapeId="0" xr:uid="{17F11297-B4B3-43EF-885F-63C67323F0DB}">
       <text>
-        <t>[Kommentarthread]
-Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
-Kommentar:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     Protein -or- Metabolite</t>
       </text>
     </comment>
     <comment ref="B3" authorId="2" shapeId="0" xr:uid="{4322AA84-C7CC-4354-AC22-60E4336DF3E7}">
       <text>
-        <t>[Kommentarthread]
-Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
-Kommentar:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     Describes the quantification technique used for your sample.
 Note: Choose between the following:
 - 180
@@ -91,65 +91,65 @@
     </comment>
     <comment ref="E3" authorId="3" shapeId="0" xr:uid="{E3D92B8D-BA9E-4821-ABA1-57F308895F9E}">
       <text>
-        <t>[Kommentarthread]
-Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
-Kommentar:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     Name of the peptidase used for digestion (e.g. 'trypsin').</t>
       </text>
     </comment>
     <comment ref="H3" authorId="4" shapeId="0" xr:uid="{1265673D-A414-4AE5-8FEE-6881C96C44D9}">
       <text>
-        <t>[Kommentarthread]
-Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
-Kommentar:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     The type of molecule you are investigating (e.g. 'protein' or 'peptide').</t>
       </text>
     </comment>
     <comment ref="K3" authorId="5" shapeId="0" xr:uid="{C8084950-78A9-4551-98E4-C248007EA43A}">
       <text>
-        <t>[Kommentarthread]
-Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
-Kommentar:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     The state in which your sample is (e.g. 'solution' or 'suspension').</t>
       </text>
     </comment>
     <comment ref="N3" authorId="6" shapeId="0" xr:uid="{AE0CB0ED-70E0-4DDF-B26D-7AF05B2AF85E}">
       <text>
-        <t>[Kommentarthread]
-Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
-Kommentar:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     The staining method applied to the sample (e.g. Coomassie staining).</t>
       </text>
     </comment>
     <comment ref="Q3" authorId="7" shapeId="0" xr:uid="{F5716B7C-2907-4CE9-B9AF-2116E274CCF7}">
       <text>
-        <t>[Kommentarthread]
-Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
-Kommentar:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     The name of composition of the buffer you applied to the sample (e.g. 'Tris').</t>
       </text>
     </comment>
     <comment ref="T3" authorId="8" shapeId="0" xr:uid="{7B9B508E-A99F-4AD9-8593-43D9510F63FF}">
       <text>
-        <t>[Kommentarthread]
-Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
-Kommentar:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     The pH of the sample (e.g. '7').</t>
       </text>
     </comment>
     <comment ref="Z3" authorId="9" shapeId="0" xr:uid="{2EF25143-3A7C-410B-9605-29381ABFAB67}">
       <text>
-        <t>[Kommentarthread]
-Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
-Kommentar:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     The fractionation technique applied to the sample (e.g. 'SCX').</t>
       </text>
     </comment>
     <comment ref="AC3" authorId="10" shapeId="0" xr:uid="{4F6E06A1-AA9E-439F-872A-513CC000BE80}">
       <text>
-        <t>[Kommentarthread]
-Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
-Kommentar:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     The sample deslating and seperation method used (e.g. 'C18').</t>
       </text>
     </comment>
@@ -393,7 +393,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="9">
     <dxf>
@@ -443,7 +443,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{6D6A5A68-C33B-42E1-9BA0-0CF433F987F9}" name="annotationTable3" displayName="annotationTable3" ref="A3:AF4" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{6D6A5A68-C33B-42E1-9BA0-0CF433F987F9}" name="annotationTable" displayName="annotationTable" ref="A3:AF4" totalsRowShown="0">
   <autoFilter ref="A3:AF4" xr:uid="{9ED13356-DBC8-4ADA-9EB3-EC237093C08B}"/>
   <tableColumns count="32">
     <tableColumn id="1" xr3:uid="{6C2FF147-5B29-4B17-88EA-BB5AFE8A67F6}" name="Source Name"/>
@@ -484,7 +484,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -835,7 +835,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="619" row="0">
+  <wetp:taskpane dockstate="right" visibility="0" width="633" row="2">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -856,46 +856,46 @@
   <dimension ref="A1:AF4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.7109375" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="51.7109375" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="33.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="56.5703125" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="63.5703125" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.86328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.1328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.73046875" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="51.73046875" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="33.3984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="56.59765625" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="63.59765625" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="22.86328125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="46" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="53" hidden="1" customWidth="1"/>
     <col min="11" max="11" width="26" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="49" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="56.140625" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="56.1328125" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="21.59765625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="45" hidden="1" customWidth="1"/>
     <col min="16" max="16" width="52" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="43.42578125" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="50.5703125" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.1328125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="43.3984375" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="50.59765625" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="16.86328125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="40" hidden="1" customWidth="1"/>
     <col min="22" max="22" width="47" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="32.140625" hidden="1" customWidth="1"/>
-    <col min="24" max="24" width="43.140625" hidden="1" customWidth="1"/>
-    <col min="25" max="25" width="50.28515625" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="32.1328125" hidden="1" customWidth="1"/>
+    <col min="24" max="24" width="43.1328125" hidden="1" customWidth="1"/>
+    <col min="25" max="25" width="50.265625" hidden="1" customWidth="1"/>
     <col min="26" max="26" width="37" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="60.140625" hidden="1" customWidth="1"/>
-    <col min="28" max="28" width="67.140625" hidden="1" customWidth="1"/>
-    <col min="29" max="29" width="28.28515625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="51.7109375" hidden="1" customWidth="1"/>
-    <col min="31" max="31" width="58.7109375" hidden="1" customWidth="1"/>
-    <col min="32" max="32" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="60.1328125" hidden="1" customWidth="1"/>
+    <col min="28" max="28" width="67.1328125" hidden="1" customWidth="1"/>
+    <col min="29" max="29" width="28.265625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="51.73046875" hidden="1" customWidth="1"/>
+    <col min="31" max="31" width="58.73046875" hidden="1" customWidth="1"/>
+    <col min="32" max="32" width="15.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" hidden="1" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>10</v>
       </c>
@@ -927,7 +927,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A2" s="5"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -961,7 +961,7 @@
       <c r="AE2" s="6"/>
       <c r="AF2" s="7"/>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1059,7 +1059,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.45">
       <c r="B4" s="1"/>
       <c r="E4" s="1"/>
       <c r="H4" s="1"/>
@@ -1081,43 +1081,9 @@
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <customXml>
-  <SwateTable Table="annotationTable2" Worksheet="Data procession">
-    <TableValidation DateTime="2021-03-02 14:11" SwateVersion="0.4.0" TableName="annotationTable2" Userlist="" WorksheetName="Data procession">
-      <ColumnValidation ColumnAdress="0" ColumnHeader="Source Name" Importance="5" Unit="None" ValidationFormat="Text"/>
-      <ColumnValidation ColumnAdress="1" ColumnHeader="Parameter [acquisition software]" Importance="3" Unit="None" ValidationFormat="OntologyTerm acquisition software"/>
-      <ColumnValidation ColumnAdress="4" ColumnHeader="Parameter [analysis software]" Importance="3" Unit="None" ValidationFormat="OntologyTerm analysis software"/>
-      <ColumnValidation ColumnAdress="7" ColumnHeader="Parameter [data processing software]" Importance="3" Unit="None" ValidationFormat="OntologyTerm data processing software"/>
-      <ColumnValidation ColumnAdress="10" ColumnHeader="Data File Name" Importance="5" Unit="None" ValidationFormat="Text"/>
-    </TableValidation>
-  </SwateTable>
-  <SwateTable Table="annotationTable1" Worksheet="Measurement">
-    <TableValidation DateTime="2021-03-02 14:10" SwateVersion="0.4.0" TableName="annotationTable1" Userlist="" WorksheetName="Measurement">
-      <ColumnValidation ColumnAdress="0" ColumnHeader="Source Name" Importance="5" Unit="None" ValidationFormat="Text"/>
-      <ColumnValidation ColumnAdress="1" ColumnHeader="Parameter [technical replicate]" Importance="3" Unit="None" ValidationFormat="Int"/>
-      <ColumnValidation ColumnAdress="4" ColumnHeader="Parameter [Variable modification]" Importance="4" Unit="None" ValidationFormat="OntologyTerm Variable modification"/>
-      <ColumnValidation ColumnAdress="7" ColumnHeader="Parameter [Fixed modification]" Importance="4" Unit="None" ValidationFormat="OntologyTerm Fixed modification"/>
-      <ColumnValidation ColumnAdress="10" ColumnHeader="Parameter [sample volume]" Importance="2" Unit="None" ValidationFormat="Number"/>
-      <ColumnValidation ColumnAdress="13" ColumnHeader="Parameter [injection volume]" Importance="2" Unit="None" ValidationFormat="Number"/>
-      <ColumnValidation ColumnAdress="16" ColumnHeader="Parameter [count unit]" Importance="3" Unit="None" ValidationFormat="Int"/>
-      <ColumnValidation ColumnAdress="19" ColumnHeader="Parameter [instrument model]" Importance="3" Unit="None" ValidationFormat="OntologyTerm instrument model"/>
-      <ColumnValidation ColumnAdress="22" ColumnHeader="Parameter [duration]" Importance="4" Unit="None" ValidationFormat="Number"/>
-      <ColumnValidation ColumnAdress="25" ColumnHeader="Data File Name" Importance="5" Unit="None" ValidationFormat="Text"/>
-    </TableValidation>
-  </SwateTable>
-  <SwateTable Table="annotationTable" Worksheet="Sample preparation">
-    <TableValidation DateTime="2021-03-02 14:07" SwateVersion="0.4.0" TableName="annotationTable" Userlist="" WorksheetName="Sample preparation">
-      <ColumnValidation ColumnAdress="0" ColumnHeader="Source Name" Importance="5" Unit="None" ValidationFormat="Text"/>
-      <ColumnValidation ColumnAdress="1" ColumnHeader="Characteristics [species]" Importance="4" Unit="None" ValidationFormat="OntologyTerm species"/>
-      <ColumnValidation ColumnAdress="4" ColumnHeader="Characteristics [genotype information]" Importance="4" Unit="None" ValidationFormat="OntologyTerm genotype information"/>
-      <ColumnValidation ColumnAdress="7" ColumnHeader="Characteristics [sample preparation]" Importance="5" Unit="None" ValidationFormat="OntologyTerm sample preparation"/>
-      <ColumnValidation ColumnAdress="10" ColumnHeader="Characteristics [protein tag]" Importance="3" Unit="None" ValidationFormat="OntologyTerm protein tag"/>
-      <ColumnValidation ColumnAdress="13" ColumnHeader="Characteristics [tissues, cell types and enzyme sources]" Importance="2" Unit="None" ValidationFormat="OntologyTerm tissues, cell types and enzyme sources"/>
-      <ColumnValidation ColumnAdress="16" ColumnHeader="Characteristics [cell]" Importance="3" Unit="None" ValidationFormat="OntologyTerm cell"/>
-      <ColumnValidation ColumnAdress="19" ColumnHeader="Characteristics [disease]" Importance="1" Unit="None" ValidationFormat="OntologyTerm disease"/>
-      <ColumnValidation ColumnAdress="22" ColumnHeader="Characteristics [biological replicate]" Importance="2" Unit="None" ValidationFormat="Int"/>
+  <SwateTable Table="annotationTable" Worksheet="2EXT02_ProteomicsExtraction">
+    <TableValidation DateTime="2021-03-02 14:07" SwateVersion="0.4.4" TableName="annotationTable" Userlist="" WorksheetName="2EXT02_ProteomicsExtraction">
       <ColumnValidation ColumnAdress="25" ColumnHeader="Parameter [Quantification method]" Importance="3" Unit="None" ValidationFormat="OntologyTerm Quantification method"/>
-      <ColumnValidation ColumnAdress="28" ColumnHeader="Parameter [spectrum interpretation]" Importance="3" Unit="None" ValidationFormat="OntologyTerm spectrum interpretation"/>
-      <ColumnValidation ColumnAdress="31" ColumnHeader="Parameter [matrix solution]" Importance="2" Unit="None" ValidationFormat="OntologyTerm matrix solution"/>
       <ColumnValidation ColumnAdress="34" ColumnHeader="Parameter [cleavage agent name]" Importance="3" Unit="None" ValidationFormat="OntologyTerm cleavage agent name"/>
       <ColumnValidation ColumnAdress="37" ColumnHeader="Parameter [molecule]" Importance="3" Unit="None" ValidationFormat="OntologyTerm molecule"/>
       <ColumnValidation ColumnAdress="40" ColumnHeader="Parameter [sample state]" Importance="2" Unit="None" ValidationFormat="OntologyTerm sample state"/>
@@ -1126,8 +1092,6 @@
       <ColumnValidation ColumnAdress="49" ColumnHeader="Parameter [ph]" Importance="2" Unit="None" ValidationFormat="Number"/>
       <ColumnValidation ColumnAdress="52" ColumnHeader="Parameter [sample pre-fractionation]" Importance="3" Unit="None" ValidationFormat="OntologyTerm sample pre-fractionation"/>
       <ColumnValidation ColumnAdress="55" ColumnHeader="Parameter [protein column]" Importance="3" Unit="None" ValidationFormat="OntologyTerm protein column"/>
-      <ColumnValidation ColumnAdress="58" ColumnHeader="Parameter [temperature]" Importance="3" Unit="degree Celsius" ValidationFormat="UnitTerm degree Celsius"/>
-      <ColumnValidation ColumnAdress="64" ColumnHeader="Parameter [time]" Importance="3" Unit="None" ValidationFormat="Number"/>
       <ColumnValidation ColumnAdress="67" ColumnHeader="Sample Name" Importance="5" Unit="None" ValidationFormat="Text"/>
     </TableValidation>
   </SwateTable>
@@ -1135,7 +1099,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC659FA7-EECD-4F3A-A590-22A36420F9C2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F5E3DB9-4ECA-435D-9C07-1D3ACBAFA05D}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
</xml_diff>